<commit_message>
Corrected errors in fire, wind and mech remove scripts and values
</commit_message>
<xml_diff>
--- a/specifications/DisturbanceCodes.xlsx
+++ b/specifications/DisturbanceCodes.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\FuelbedMapping\datafiles-fuelbedmapping\LANDFIRE\LF_disturbance_update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\LANDFIRE\landfiredisturbance-clone\specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27780" windowHeight="13860"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ExpectedTrends" sheetId="2" r:id="rId1"/>
+    <sheet name="Codes" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="56">
   <si>
     <t>Type</t>
   </si>
@@ -138,6 +139,60 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Shrub</t>
+  </si>
+  <si>
+    <t>Herb</t>
+  </si>
+  <si>
+    <t>LLM</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Slight reduction</t>
+  </si>
+  <si>
+    <t>No change</t>
+  </si>
+  <si>
+    <t>Canopy-trees</t>
+  </si>
+  <si>
+    <t>Canopy-Snags</t>
+  </si>
+  <si>
+    <t>Slight increase</t>
+  </si>
+  <si>
+    <t>Reduction</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
+  <si>
+    <t>Restored</t>
+  </si>
+  <si>
+    <t>Wood-fine</t>
+  </si>
+  <si>
+    <t>Wood-coarse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase </t>
+  </si>
+  <si>
+    <t>Wood-stumps</t>
+  </si>
+  <si>
+    <t>no change</t>
+  </si>
+  <si>
+    <t>No change or increase</t>
   </si>
 </sst>
 </file>
@@ -561,10 +616,1716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>123</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>132</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>133</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>49</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>211</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>212</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>213</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>221</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>222</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" t="s">
+        <v>43</v>
+      </c>
+      <c r="M16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>223</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>231</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>232</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>233</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>311</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J22" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L22" t="s">
+        <v>47</v>
+      </c>
+      <c r="M22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>312</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>313</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" t="s">
+        <v>49</v>
+      </c>
+      <c r="J24" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>321</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" t="s">
+        <v>48</v>
+      </c>
+      <c r="L25" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>322</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L26" t="s">
+        <v>48</v>
+      </c>
+      <c r="M26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>323</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L27" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>331</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
+      <c r="K28" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>332</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L29" t="s">
+        <v>48</v>
+      </c>
+      <c r="M29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>333</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" t="s">
+        <v>43</v>
+      </c>
+      <c r="K30" t="s">
+        <v>43</v>
+      </c>
+      <c r="L30" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>411</v>
+      </c>
+      <c r="E32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" t="s">
+        <v>43</v>
+      </c>
+      <c r="L32" t="s">
+        <v>48</v>
+      </c>
+      <c r="M32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>412</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" t="s">
+        <v>43</v>
+      </c>
+      <c r="L33" t="s">
+        <v>43</v>
+      </c>
+      <c r="M33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>413</v>
+      </c>
+      <c r="E34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" t="s">
+        <v>47</v>
+      </c>
+      <c r="J34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K34" t="s">
+        <v>43</v>
+      </c>
+      <c r="L34" t="s">
+        <v>49</v>
+      </c>
+      <c r="M34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>421</v>
+      </c>
+      <c r="E35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" t="s">
+        <v>48</v>
+      </c>
+      <c r="J35" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" t="s">
+        <v>43</v>
+      </c>
+      <c r="L35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>422</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>423</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" t="s">
+        <v>47</v>
+      </c>
+      <c r="J37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" t="s">
+        <v>43</v>
+      </c>
+      <c r="L37" t="s">
+        <v>47</v>
+      </c>
+      <c r="M37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>431</v>
+      </c>
+      <c r="E38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" t="s">
+        <v>48</v>
+      </c>
+      <c r="M38" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>432</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I39" t="s">
+        <v>47</v>
+      </c>
+      <c r="J39" t="s">
+        <v>43</v>
+      </c>
+      <c r="K39" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" t="s">
+        <v>43</v>
+      </c>
+      <c r="M39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>433</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" t="s">
+        <v>43</v>
+      </c>
+      <c r="G40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I40" t="s">
+        <v>47</v>
+      </c>
+      <c r="J40" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" t="s">
+        <v>47</v>
+      </c>
+      <c r="M40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>511</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" t="s">
+        <v>43</v>
+      </c>
+      <c r="L42" t="s">
+        <v>43</v>
+      </c>
+      <c r="M42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>512</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" t="s">
+        <v>43</v>
+      </c>
+      <c r="I43" t="s">
+        <v>48</v>
+      </c>
+      <c r="J43" t="s">
+        <v>43</v>
+      </c>
+      <c r="K43" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" t="s">
+        <v>48</v>
+      </c>
+      <c r="M43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>513</v>
+      </c>
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" t="s">
+        <v>48</v>
+      </c>
+      <c r="J44" t="s">
+        <v>43</v>
+      </c>
+      <c r="K44" t="s">
+        <v>43</v>
+      </c>
+      <c r="L44" t="s">
+        <v>49</v>
+      </c>
+      <c r="M44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>521</v>
+      </c>
+      <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" t="s">
+        <v>43</v>
+      </c>
+      <c r="H45" t="s">
+        <v>43</v>
+      </c>
+      <c r="I45" t="s">
+        <v>43</v>
+      </c>
+      <c r="J45" t="s">
+        <v>43</v>
+      </c>
+      <c r="K45" t="s">
+        <v>43</v>
+      </c>
+      <c r="L45" t="s">
+        <v>43</v>
+      </c>
+      <c r="M45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>522</v>
+      </c>
+      <c r="E46" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" t="s">
+        <v>48</v>
+      </c>
+      <c r="J46" t="s">
+        <v>43</v>
+      </c>
+      <c r="K46" t="s">
+        <v>43</v>
+      </c>
+      <c r="L46" t="s">
+        <v>48</v>
+      </c>
+      <c r="M46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>523</v>
+      </c>
+      <c r="E47" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G47" t="s">
+        <v>43</v>
+      </c>
+      <c r="H47" t="s">
+        <v>43</v>
+      </c>
+      <c r="I47" t="s">
+        <v>48</v>
+      </c>
+      <c r="J47" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" t="s">
+        <v>43</v>
+      </c>
+      <c r="L47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>531</v>
+      </c>
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" t="s">
+        <v>43</v>
+      </c>
+      <c r="J48" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" t="s">
+        <v>43</v>
+      </c>
+      <c r="L48" t="s">
+        <v>43</v>
+      </c>
+      <c r="M48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>532</v>
+      </c>
+      <c r="E49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" t="s">
+        <v>48</v>
+      </c>
+      <c r="H49" t="s">
+        <v>48</v>
+      </c>
+      <c r="I49" t="s">
+        <v>48</v>
+      </c>
+      <c r="J49" t="s">
+        <v>43</v>
+      </c>
+      <c r="K49" t="s">
+        <v>43</v>
+      </c>
+      <c r="L49" t="s">
+        <v>48</v>
+      </c>
+      <c r="M49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>533</v>
+      </c>
+      <c r="E50" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" t="s">
+        <v>43</v>
+      </c>
+      <c r="K50" t="s">
+        <v>43</v>
+      </c>
+      <c r="L50" t="s">
+        <v>49</v>
+      </c>
+      <c r="M50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>